<commit_message>
Update Excels to match all date regions
</commit_message>
<xml_diff>
--- a/Importar MC a SOS.xlsx
+++ b/Importar MC a SOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\IVA-Compras-y-Ventas-PDF-y-TXT-de-LID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E086D8ED-293E-4F5E-9E2B-3EA9E670DED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF91157-C208-4148-B481-21A472E0DEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1608,9 +1608,7 @@
         <row r="57">
           <cell r="G57"/>
           <cell r="H57"/>
-          <cell r="I57">
-            <v>1</v>
-          </cell>
+          <cell r="I57"/>
         </row>
         <row r="58">
           <cell r="G58"/>
@@ -1620,26 +1618,26 @@
           </cell>
         </row>
         <row r="59">
-          <cell r="G59" t="str">
-            <v>federico.a@elvascosa.com.ar</v>
-          </cell>
+          <cell r="G59"/>
           <cell r="H59"/>
           <cell r="I59">
-            <v>4</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="60">
-          <cell r="G60"/>
+          <cell r="G60" t="str">
+            <v>federico.a@elvascosa.com.ar</v>
+          </cell>
           <cell r="H60"/>
           <cell r="I60">
-            <v>2</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="61">
           <cell r="G61"/>
           <cell r="H61"/>
           <cell r="I61">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="62">
@@ -1653,37 +1651,37 @@
           <cell r="G63"/>
           <cell r="H63"/>
           <cell r="I63">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="64">
-          <cell r="G64" t="str">
-            <v>federico.a@elvascosa.com.ar</v>
-          </cell>
+          <cell r="G64"/>
           <cell r="H64"/>
           <cell r="I64">
-            <v>5</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="65">
-          <cell r="G65"/>
+          <cell r="G65" t="str">
+            <v>federico.a@elvascosa.com.ar</v>
+          </cell>
           <cell r="H65"/>
           <cell r="I65">
-            <v>1</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="66">
           <cell r="G66"/>
           <cell r="H66"/>
           <cell r="I66">
-            <v>2</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="67">
           <cell r="G67"/>
           <cell r="H67"/>
           <cell r="I67">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="68">
@@ -1703,17 +1701,21 @@
         <row r="70">
           <cell r="G70"/>
           <cell r="H70"/>
+          <cell r="I70">
+            <v>1</v>
+          </cell>
         </row>
         <row r="71">
           <cell r="G71"/>
           <cell r="H71"/>
-          <cell r="I71">
-            <v>1</v>
-          </cell>
+          <cell r="I71"/>
         </row>
         <row r="72">
           <cell r="G72"/>
           <cell r="H72"/>
+          <cell r="I72">
+            <v>1</v>
+          </cell>
         </row>
         <row r="73">
           <cell r="G73"/>
@@ -1722,9 +1724,7 @@
         <row r="74">
           <cell r="G74"/>
           <cell r="H74"/>
-          <cell r="I74">
-            <v>1</v>
-          </cell>
+          <cell r="I74"/>
         </row>
         <row r="75">
           <cell r="G75"/>
@@ -1736,7 +1736,9 @@
         <row r="76">
           <cell r="G76"/>
           <cell r="H76"/>
-          <cell r="I76"/>
+          <cell r="I76">
+            <v>1</v>
+          </cell>
         </row>
         <row r="77">
           <cell r="G77"/>
@@ -1746,28 +1748,26 @@
         <row r="78">
           <cell r="G78"/>
           <cell r="H78"/>
-          <cell r="I78">
-            <v>2</v>
-          </cell>
+          <cell r="I78"/>
         </row>
         <row r="79">
           <cell r="G79"/>
           <cell r="H79"/>
           <cell r="I79">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="80">
-          <cell r="G80" t="str">
-            <v>maarupensa@hotmail.com</v>
-          </cell>
+          <cell r="G80"/>
           <cell r="H80"/>
           <cell r="I80">
             <v>1</v>
           </cell>
         </row>
         <row r="81">
-          <cell r="G81"/>
+          <cell r="G81" t="str">
+            <v>maarupensa@hotmail.com</v>
+          </cell>
           <cell r="H81"/>
           <cell r="I81">
             <v>1</v>
@@ -1802,27 +1802,25 @@
           </cell>
         </row>
         <row r="86">
-          <cell r="G86" t="str">
+          <cell r="G86"/>
+          <cell r="H86"/>
+          <cell r="I86">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="G87" t="str">
             <v>maarupensa@hotmail.com</v>
           </cell>
-          <cell r="H86" t="str">
+          <cell r="H87" t="str">
             <v>lucianoanibalpensa@gmail.com</v>
           </cell>
-          <cell r="I86">
+          <cell r="I87">
             <v>2</v>
           </cell>
         </row>
-        <row r="87">
-          <cell r="G87"/>
-          <cell r="H87"/>
-          <cell r="I87">
-            <v>1</v>
-          </cell>
-        </row>
         <row r="88">
-          <cell r="G88" t="str">
-            <v>ejpere@yahoo.com.ar</v>
-          </cell>
+          <cell r="G88"/>
           <cell r="H88"/>
           <cell r="I88">
             <v>1</v>
@@ -1830,7 +1828,7 @@
         </row>
         <row r="89">
           <cell r="G89" t="str">
-            <v>jorgefpianesi@hotmail.com</v>
+            <v>ejpere@yahoo.com.ar</v>
           </cell>
           <cell r="H89"/>
           <cell r="I89">
@@ -1838,7 +1836,9 @@
           </cell>
         </row>
         <row r="90">
-          <cell r="G90"/>
+          <cell r="G90" t="str">
+            <v>jorgefpianesi@hotmail.com</v>
+          </cell>
           <cell r="H90"/>
           <cell r="I90">
             <v>1</v>
@@ -1848,27 +1848,27 @@
           <cell r="G91"/>
           <cell r="H91"/>
           <cell r="I91">
-            <v>2</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="92">
           <cell r="G92"/>
           <cell r="H92"/>
           <cell r="I92">
-            <v>4</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="93">
-          <cell r="G93" t="str">
-            <v>administracion@consalud.com.ar</v>
-          </cell>
+          <cell r="G93"/>
           <cell r="H93"/>
           <cell r="I93">
-            <v>1</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="94">
-          <cell r="G94"/>
+          <cell r="G94" t="str">
+            <v>administracion@consalud.com.ar</v>
+          </cell>
           <cell r="H94"/>
           <cell r="I94">
             <v>1</v>
@@ -1913,7 +1913,7 @@
           <cell r="G100"/>
           <cell r="H100"/>
           <cell r="I100">
-            <v>2</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="101">
@@ -1924,27 +1924,28 @@
           </cell>
         </row>
         <row r="102">
-          <cell r="G102" t="str">
+          <cell r="G102"/>
+          <cell r="H102"/>
+          <cell r="I102">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="G103" t="str">
             <v>juanlaudin@gmail.com</v>
           </cell>
-          <cell r="H102"/>
-        </row>
-        <row r="103">
-          <cell r="G103"/>
           <cell r="H103"/>
         </row>
         <row r="104">
-          <cell r="G104" t="str">
+          <cell r="G104"/>
+          <cell r="H104"/>
+        </row>
+        <row r="105">
+          <cell r="G105" t="str">
             <v>juanlaudin@gmail.com</v>
           </cell>
-          <cell r="H104"/>
-        </row>
-        <row r="105">
-          <cell r="G105"/>
           <cell r="H105"/>
-          <cell r="I105">
-            <v>1</v>
-          </cell>
+          <cell r="I105"/>
         </row>
         <row r="106">
           <cell r="G106"/>
@@ -1964,55 +1965,55 @@
           <cell r="G108"/>
           <cell r="H108"/>
           <cell r="I108">
-            <v>2</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="109">
           <cell r="G109"/>
           <cell r="H109"/>
           <cell r="I109">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="110">
           <cell r="G110"/>
           <cell r="H110"/>
           <cell r="I110">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="G111"/>
+          <cell r="H111"/>
+          <cell r="I111">
             <v>2</v>
           </cell>
         </row>
-        <row r="111">
-          <cell r="G111" t="str">
+        <row r="112">
+          <cell r="G112" t="str">
             <v>jcamarilla@hotmail.com</v>
           </cell>
-          <cell r="H111" t="str">
+          <cell r="H112" t="str">
             <v>molinosfabiola@gmail.com</v>
           </cell>
-          <cell r="I111">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="G112"/>
-          <cell r="H112"/>
           <cell r="I112">
             <v>1</v>
           </cell>
         </row>
         <row r="113">
-          <cell r="G113" t="str">
-            <v>carlosandresferreyra17@gmail.com</v>
-          </cell>
+          <cell r="G113"/>
           <cell r="H113"/>
           <cell r="I113">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="114">
-          <cell r="G114"/>
+          <cell r="G114" t="str">
+            <v>carlosandresferreyra17@gmail.com</v>
+          </cell>
           <cell r="H114"/>
           <cell r="I114">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="115">
@@ -2023,16 +2024,16 @@
           </cell>
         </row>
         <row r="116">
-          <cell r="G116" t="str">
-            <v>diegoau911@hotmail.com</v>
-          </cell>
+          <cell r="G116"/>
           <cell r="H116"/>
           <cell r="I116">
             <v>1</v>
           </cell>
         </row>
         <row r="117">
-          <cell r="G117"/>
+          <cell r="G117" t="str">
+            <v>diegoau911@hotmail.com</v>
+          </cell>
           <cell r="H117"/>
           <cell r="I117">
             <v>1</v>
@@ -2046,37 +2047,44 @@
           </cell>
         </row>
         <row r="119">
-          <cell r="G119" t="str">
-            <v>male_432@hotmail.com</v>
-          </cell>
+          <cell r="G119"/>
           <cell r="H119"/>
           <cell r="I119">
             <v>1</v>
           </cell>
         </row>
         <row r="120">
-          <cell r="G120"/>
+          <cell r="G120" t="str">
+            <v>male_432@hotmail.com</v>
+          </cell>
           <cell r="H120"/>
           <cell r="I120">
             <v>1</v>
           </cell>
         </row>
         <row r="121">
-          <cell r="G121" t="str">
-            <v>varenizaleo@gmail.com</v>
-          </cell>
+          <cell r="G121"/>
           <cell r="H121"/>
           <cell r="I121">
             <v>1</v>
           </cell>
         </row>
         <row r="122">
-          <cell r="G122"/>
+          <cell r="G122" t="str">
+            <v>varenizaleo@gmail.com</v>
+          </cell>
           <cell r="H122"/>
+          <cell r="I122">
+            <v>1</v>
+          </cell>
         </row>
         <row r="123">
           <cell r="G123"/>
           <cell r="H123"/>
+        </row>
+        <row r="124">
+          <cell r="G124"/>
+          <cell r="H124"/>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
@@ -2387,7 +2395,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,6 +2408,7 @@
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
     <col min="12" max="13" width="16.5703125" customWidth="1"/>
     <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.85546875" hidden="1" customWidth="1"/>
@@ -2499,23 +2508,23 @@
         <v>44985</v>
       </c>
       <c r="K2" s="3" t="str">
-        <f t="shared" ref="K2:K33" si="2">TEXT(F2,"DD/MM/AAAA")</f>
+        <f>TEXT(DAY(F2),"00")&amp;"/"&amp;TEXT(MONTH(F2),"00")&amp;"/"&amp;YEAR(F2)</f>
         <v>01/02/2023</v>
       </c>
       <c r="L2" s="3" t="str">
-        <f t="shared" ref="L2:L33" si="3">TEXT(J2,"DD/MM/AAAA")</f>
+        <f>TEXT(DAY(J2),"00")&amp;"/"&amp;TEXT(MONTH(J2),"00")&amp;"/"&amp;YEAR(J2)</f>
         <v>28/02/2023</v>
       </c>
       <c r="M2" s="3" t="str">
-        <f t="shared" ref="M2:M33" si="4">CONCATENATE(A2," - ","MCE - ",TEXT(K2,"AAAAMM")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
+        <f>CONCATENATE(A2," - ","MCE - ",U2," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
         <v>0 - MCE - 202302 - 20168291680 - CRIVELLO LUIS</v>
       </c>
       <c r="N2" s="3" t="str">
-        <f t="shared" ref="N2:N33" si="5">CONCATENATE(A2," - ","MCR - ",TEXT(K2,"AAAAMM")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
+        <f>CONCATENATE(A2," - ","MCR - ",U2," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
         <v>0 - MCR - 202302 - 20168291680 - CRIVELLO LUIS</v>
       </c>
       <c r="O2" s="1" t="str">
-        <f t="shared" ref="O2:O33" si="6">TEXT(R2+S2/96400,"hh:mm:ss")</f>
+        <f t="shared" ref="O2:O33" si="2">TEXT(R2+S2/96400,"hh:mm:ss")</f>
         <v>00:00:03</v>
       </c>
       <c r="P2" s="1" t="e">
@@ -2523,7 +2532,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q2" s="6" t="e">
-        <f t="shared" ref="Q2:Q33" si="7">IF(EXACT(P2,E2),"ü","x")</f>
+        <f t="shared" ref="Q2:Q33" si="3">IF(EXACT(P2,E2),"ü","x")</f>
         <v>#N/A</v>
       </c>
       <c r="R2" s="7" t="s">
@@ -2533,11 +2542,11 @@
         <v>2</v>
       </c>
       <c r="T2" s="1">
-        <f t="shared" ref="T2:T33" si="8">ROW(A2)</f>
-        <v>2</v>
-      </c>
-      <c r="U2" s="1" t="str">
-        <f t="shared" ref="U2:U33" si="9">TEXT(K2,"AAAAMM")</f>
+        <f t="shared" ref="T2:T33" si="4">ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="U2" s="3" t="str">
+        <f>YEAR(F2)&amp;TEXT(MONTH(F2),"00")</f>
         <v>202302</v>
       </c>
     </row>
@@ -2565,27 +2574,27 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J3:J66" si="5">EOMONTH(F3,0)</f>
         <v>44985</v>
       </c>
       <c r="K3" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K3:K66" si="6">TEXT(DAY(F3),"00")&amp;"/"&amp;TEXT(MONTH(F3),"00")&amp;"/"&amp;YEAR(F3)</f>
         <v>01/02/2023</v>
       </c>
       <c r="L3" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="L3:L66" si="7">TEXT(DAY(J3),"00")&amp;"/"&amp;TEXT(MONTH(J3),"00")&amp;"/"&amp;YEAR(J3)</f>
         <v>28/02/2023</v>
       </c>
       <c r="M3" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="M3:M66" si="8">CONCATENATE(A3," - ","MCE - ",U3," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
         <v>0 - MCE - 202302 - 20315731330 - VARENIZA ANGEL</v>
       </c>
       <c r="N3" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="N3:N66" si="9">CONCATENATE(A3," - ","MCR - ",U3," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
         <v>0 - MCR - 202302 - 20315731330 - VARENIZA ANGEL</v>
       </c>
       <c r="O3" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="O3:O66" si="10">TEXT(R3+S3/96400,"hh:mm:ss")</f>
         <v>00:00:03</v>
       </c>
       <c r="P3" s="1" t="e">
@@ -2593,7 +2602,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q3" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="Q3:Q66" si="11">IF(EXACT(P3,E3),"ü","x")</f>
         <v>#N/A</v>
       </c>
       <c r="R3" s="7" t="s">
@@ -2603,11 +2612,11 @@
         <v>2</v>
       </c>
       <c r="T3" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="T3:T66" si="12">ROW(A3)</f>
         <v>3</v>
       </c>
-      <c r="U3" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U3" s="3" t="str">
+        <f t="shared" ref="U3:U66" si="13">YEAR(F3)&amp;TEXT(MONTH(F3),"00")</f>
         <v>202302</v>
       </c>
     </row>
@@ -2635,27 +2644,27 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K4" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L4" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M4" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202302 - 27067089680 - SESMERO DORA TERESITA</v>
       </c>
       <c r="N4" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202302 - 27067089680 - SESMERO DORA TERESITA</v>
       </c>
       <c r="O4" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P4" s="1" t="e">
@@ -2663,7 +2672,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q4" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R4" s="7" t="s">
@@ -2673,11 +2682,11 @@
         <v>2</v>
       </c>
       <c r="T4" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="U4" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U4" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -2705,27 +2714,27 @@
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K5" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L5" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M5" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202302 - 27116976620 - URRUTIA MIRIAM</v>
       </c>
       <c r="N5" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202302 - 27116976620 - URRUTIA MIRIAM</v>
       </c>
       <c r="O5" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P5" s="1" t="e">
@@ -2733,7 +2742,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q5" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R5" s="7" t="s">
@@ -2743,11 +2752,11 @@
         <v>2</v>
       </c>
       <c r="T5" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="U5" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U5" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -2774,27 +2783,27 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K6" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L6" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M6" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0 - MCE - 202302 - 30657146850 - MEDINT SRL</v>
       </c>
       <c r="N6" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0 - MCR - 202302 - 30657146850 - MEDINT SRL</v>
       </c>
       <c r="O6" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P6" s="1" t="e">
@@ -2802,7 +2811,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q6" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R6" s="7" t="s">
@@ -2812,11 +2821,11 @@
         <v>2</v>
       </c>
       <c r="T6" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
-      <c r="U6" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U6" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -2843,27 +2852,27 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K7" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L7" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M7" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1 - MCE - 202302 - 20133762761 - FERREYRA CARLOS ALFREDO</v>
       </c>
       <c r="N7" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1 - MCR - 202302 - 20133762761 - FERREYRA CARLOS ALFREDO</v>
       </c>
       <c r="O7" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P7" s="1" t="e">
@@ -2871,7 +2880,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q7" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R7" s="7" t="s">
@@ -2881,11 +2890,11 @@
         <v>2</v>
       </c>
       <c r="T7" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
-      <c r="U7" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U7" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -2912,27 +2921,27 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K8" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L8" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M8" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1 - MCE - 202302 - 20149462601 - SZYCHOWSKI MARCELO</v>
       </c>
       <c r="N8" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1 - MCR - 202302 - 20149462601 - SZYCHOWSKI MARCELO</v>
       </c>
       <c r="O8" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P8" s="1" t="e">
@@ -2940,7 +2949,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q8" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R8" s="7" t="s">
@@ -2950,11 +2959,11 @@
         <v>2</v>
       </c>
       <c r="T8" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
-      <c r="U8" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U8" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -2982,27 +2991,27 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K9" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L9" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M9" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1 - MCE - 202302 - 20168291281 - BUSTOS GUSTAVO</v>
       </c>
       <c r="N9" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1 - MCR - 202302 - 20168291281 - BUSTOS GUSTAVO</v>
       </c>
       <c r="O9" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P9" s="1" t="e">
@@ -3010,7 +3019,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q9" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R9" s="7" t="s">
@@ -3020,11 +3029,11 @@
         <v>2</v>
       </c>
       <c r="T9" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="U9" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U9" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3052,27 +3061,27 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K10" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L10" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M10" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1 - MCE - 202302 - 20172521771 - PEREYRA ESTEBAN</v>
       </c>
       <c r="N10" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1 - MCR - 202302 - 20172521771 - PEREYRA ESTEBAN</v>
       </c>
       <c r="O10" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P10" s="1" t="e">
@@ -3080,7 +3089,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q10" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R10" s="7" t="s">
@@ -3090,11 +3099,11 @@
         <v>2</v>
       </c>
       <c r="T10" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
-      <c r="U10" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U10" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3122,27 +3131,27 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K11" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L11" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M11" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1 - MCE - 202302 - 27128520851 - MOLAS CARMEN PATRICIA</v>
       </c>
       <c r="N11" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1 - MCR - 202302 - 27128520851 - MOLAS CARMEN PATRICIA</v>
       </c>
       <c r="O11" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P11" s="1" t="e">
@@ -3150,7 +3159,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q11" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R11" s="7" t="s">
@@ -3160,11 +3169,11 @@
         <v>2</v>
       </c>
       <c r="T11" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
-      <c r="U11" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U11" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3197,27 +3206,27 @@
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44773</v>
       </c>
       <c r="K12" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/07/2022</v>
       </c>
       <c r="L12" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>31/07/2022</v>
       </c>
       <c r="M12" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1 - MCE - 202207 - 30710404131 - GESAL SA</v>
       </c>
       <c r="N12" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1 - MCR - 202207 - 30710404131 - GESAL SA</v>
       </c>
       <c r="O12" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P12" s="1" t="e">
@@ -3225,7 +3234,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q12" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R12" s="7" t="s">
@@ -3235,11 +3244,11 @@
         <v>2</v>
       </c>
       <c r="T12" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
-      <c r="U12" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U12" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202207</v>
       </c>
     </row>
@@ -3266,27 +3275,27 @@
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K13" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L13" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M13" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1 - MCE - 202302 - 30717059111 - CONDOMINIO SAN LORENZO</v>
       </c>
       <c r="N13" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1 - MCR - 202302 - 30717059111 - CONDOMINIO SAN LORENZO</v>
       </c>
       <c r="O13" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P13" s="1" t="e">
@@ -3294,7 +3303,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q13" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R13" s="7" t="s">
@@ -3304,11 +3313,11 @@
         <v>2</v>
       </c>
       <c r="T13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
-      <c r="U13" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U13" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3336,27 +3345,27 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K14" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L14" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M14" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2 - MCE - 202302 - 20121182832 - RIERA HECTOR MANUEL</v>
       </c>
       <c r="N14" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2 - MCR - 202302 - 20121182832 - RIERA HECTOR MANUEL</v>
       </c>
       <c r="O14" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P14" s="1" t="e">
@@ -3364,7 +3373,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q14" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R14" s="7" t="s">
@@ -3374,11 +3383,11 @@
         <v>2</v>
       </c>
       <c r="T14" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
-      <c r="U14" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U14" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3406,27 +3415,27 @@
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K15" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L15" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M15" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2 - MCE - 202302 - 20147130202 - BUSTOS JOSE MARTIN</v>
       </c>
       <c r="N15" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2 - MCR - 202302 - 20147130202 - BUSTOS JOSE MARTIN</v>
       </c>
       <c r="O15" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P15" s="1" t="e">
@@ -3434,7 +3443,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q15" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R15" s="7" t="s">
@@ -3444,11 +3453,11 @@
         <v>2</v>
       </c>
       <c r="T15" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
-      <c r="U15" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U15" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3475,27 +3484,27 @@
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K16" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M16" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2 - MCE - 202302 - 20174123072 - INSAURRALDE CARLOS</v>
       </c>
       <c r="N16" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2 - MCR - 202302 - 20174123072 - INSAURRALDE CARLOS</v>
       </c>
       <c r="O16" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P16" s="1" t="e">
@@ -3503,7 +3512,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q16" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R16" s="7" t="s">
@@ -3513,11 +3522,11 @@
         <v>2</v>
       </c>
       <c r="T16" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>16</v>
       </c>
-      <c r="U16" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U16" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3545,27 +3554,27 @@
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K17" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L17" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M17" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2 - MCE - 202302 - 27182653972 - FERNANDEZ SOSA LILIANA</v>
       </c>
       <c r="N17" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2 - MCR - 202302 - 27182653972 - FERNANDEZ SOSA LILIANA</v>
       </c>
       <c r="O17" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P17" s="1" t="e">
@@ -3573,7 +3582,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q17" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R17" s="7" t="s">
@@ -3583,11 +3592,11 @@
         <v>2</v>
       </c>
       <c r="T17" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>17</v>
       </c>
-      <c r="U17" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U17" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3614,27 +3623,27 @@
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K18" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L18" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M18" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2 - MCE - 202302 - 30708370122 - POSADAS FIDUCIARIA SA</v>
       </c>
       <c r="N18" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2 - MCR - 202302 - 30708370122 - POSADAS FIDUCIARIA SA</v>
       </c>
       <c r="O18" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P18" s="1" t="e">
@@ -3642,7 +3651,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q18" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R18" s="7" t="s">
@@ -3652,11 +3661,11 @@
         <v>2</v>
       </c>
       <c r="T18" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>18</v>
       </c>
-      <c r="U18" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U18" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3684,27 +3693,27 @@
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K19" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L19" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M19" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3 - MCE - 202302 - 27068286323 - SEMILLA ELVIES</v>
       </c>
       <c r="N19" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3 - MCR - 202302 - 27068286323 - SEMILLA ELVIES</v>
       </c>
       <c r="O19" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P19" s="1" t="e">
@@ -3712,7 +3721,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q19" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R19" s="7" t="s">
@@ -3722,11 +3731,11 @@
         <v>2</v>
       </c>
       <c r="T19" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>19</v>
       </c>
-      <c r="U19" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U19" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3760,27 +3769,27 @@
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44773</v>
       </c>
       <c r="K20" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/07/2022</v>
       </c>
       <c r="L20" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>31/07/2022</v>
       </c>
       <c r="M20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3 - MCE - 202207 - 27354872183 - PENSA MARIA EUGENIA</v>
       </c>
       <c r="N20" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3 - MCR - 202207 - 27354872183 - PENSA MARIA EUGENIA</v>
       </c>
       <c r="O20" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P20" s="1" t="e">
@@ -3788,7 +3797,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q20" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R20" s="7" t="s">
@@ -3798,11 +3807,11 @@
         <v>2</v>
       </c>
       <c r="T20" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
-      <c r="U20" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U20" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202207</v>
       </c>
     </row>
@@ -3829,27 +3838,27 @@
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K21" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L21" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M21" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3 - MCE - 202302 - 30707912223 - CAS SRL</v>
       </c>
       <c r="N21" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3 - MCR - 202302 - 30707912223 - CAS SRL</v>
       </c>
       <c r="O21" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P21" s="1" t="e">
@@ -3857,7 +3866,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q21" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R21" s="7" t="s">
@@ -3867,11 +3876,11 @@
         <v>2</v>
       </c>
       <c r="T21" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>21</v>
       </c>
-      <c r="U21" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U21" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -3904,27 +3913,27 @@
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44773</v>
       </c>
       <c r="K22" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/07/2022</v>
       </c>
       <c r="L22" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>31/07/2022</v>
       </c>
       <c r="M22" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3 - MCE - 202207 - 30715577743 - TRANS. MISIONES SA</v>
       </c>
       <c r="N22" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3 - MCR - 202207 - 30715577743 - TRANS. MISIONES SA</v>
       </c>
       <c r="O22" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P22" s="1" t="e">
@@ -3932,7 +3941,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q22" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R22" s="7" t="s">
@@ -3942,11 +3951,11 @@
         <v>2</v>
       </c>
       <c r="T22" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>22</v>
       </c>
-      <c r="U22" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U22" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202207</v>
       </c>
     </row>
@@ -3973,27 +3982,27 @@
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K23" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L23" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M23" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3 - MCE - 202302 - 30717537153 - DON LALO SRL</v>
       </c>
       <c r="N23" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3 - MCR - 202302 - 30717537153 - DON LALO SRL</v>
       </c>
       <c r="O23" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P23" s="1" t="e">
@@ -4001,7 +4010,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q23" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R23" s="7" t="s">
@@ -4011,11 +4020,11 @@
         <v>2</v>
       </c>
       <c r="T23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>23</v>
       </c>
-      <c r="U23" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U23" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -4043,27 +4052,27 @@
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K24" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L24" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M24" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4 - MCE - 202302 - 20168291834 - FERNADEZ SOSA RODOLFO</v>
       </c>
       <c r="N24" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4 - MCR - 202302 - 20168291834 - FERNADEZ SOSA RODOLFO</v>
       </c>
       <c r="O24" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P24" s="1" t="e">
@@ -4071,7 +4080,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q24" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R24" s="7" t="s">
@@ -4081,11 +4090,11 @@
         <v>2</v>
       </c>
       <c r="T24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>24</v>
       </c>
-      <c r="U24" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U24" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -4113,27 +4122,27 @@
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K25" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L25" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M25" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4 - MCE - 202302 - 23149462074 - SESMERO MARIA GABRIELA</v>
       </c>
       <c r="N25" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4 - MCR - 202302 - 23149462074 - SESMERO MARIA GABRIELA</v>
       </c>
       <c r="O25" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P25" s="1" t="e">
@@ -4141,7 +4150,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q25" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R25" s="7" t="s">
@@ -4151,11 +4160,11 @@
         <v>2</v>
       </c>
       <c r="T25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>25</v>
       </c>
-      <c r="U25" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U25" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -4183,27 +4192,27 @@
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K26" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L26" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M26" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4 - MCE - 202302 - 23342751644 - FERREYRA CARMEN VICTORIA</v>
       </c>
       <c r="N26" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4 - MCR - 202302 - 23342751644 - FERREYRA CARMEN VICTORIA</v>
       </c>
       <c r="O26" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P26" s="1" t="e">
@@ -4211,7 +4220,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q26" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R26" s="7" t="s">
@@ -4221,11 +4230,11 @@
         <v>2</v>
       </c>
       <c r="T26" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>26</v>
       </c>
-      <c r="U26" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U26" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -4252,27 +4261,27 @@
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K27" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L27" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M27" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4 - MCE - 202302 - 23351897074 - SCOTO LUCILA</v>
       </c>
       <c r="N27" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4 - MCR - 202302 - 23351897074 - SCOTO LUCILA</v>
       </c>
       <c r="O27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P27" s="1" t="e">
@@ -4280,7 +4289,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q27" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R27" s="7" t="s">
@@ -4290,11 +4299,11 @@
         <v>2</v>
       </c>
       <c r="T27" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>27</v>
       </c>
-      <c r="U27" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U27" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -4322,27 +4331,27 @@
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K28" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L28" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M28" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4 - MCE - 202302 - 27236873744 - TUFRO MARIA MAGDALENA</v>
       </c>
       <c r="N28" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4 - MCR - 202302 - 27236873744 - TUFRO MARIA MAGDALENA</v>
       </c>
       <c r="O28" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P28" s="1" t="e">
@@ -4350,7 +4359,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q28" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R28" s="7" t="s">
@@ -4360,11 +4369,11 @@
         <v>2</v>
       </c>
       <c r="T28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>28</v>
       </c>
-      <c r="U28" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U28" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -4397,27 +4406,27 @@
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44773</v>
       </c>
       <c r="K29" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/07/2022</v>
       </c>
       <c r="L29" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>31/07/2022</v>
       </c>
       <c r="M29" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4 - MCE - 202207 - 30709431834 - DVC SRL</v>
       </c>
       <c r="N29" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4 - MCR - 202207 - 30709431834 - DVC SRL</v>
       </c>
       <c r="O29" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P29" s="1" t="e">
@@ -4425,7 +4434,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q29" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R29" s="7" t="s">
@@ -4435,11 +4444,11 @@
         <v>2</v>
       </c>
       <c r="T29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>29</v>
       </c>
-      <c r="U29" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U29" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202207</v>
       </c>
     </row>
@@ -4466,27 +4475,27 @@
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K30" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L30" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M30" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4 - MCE - 202302 - 30715795864 - VECINAS SRL</v>
       </c>
       <c r="N30" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4 - MCR - 202302 - 30715795864 - VECINAS SRL</v>
       </c>
       <c r="O30" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P30" s="1" t="e">
@@ -4494,7 +4503,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q30" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R30" s="7" t="s">
@@ -4504,11 +4513,11 @@
         <v>2</v>
       </c>
       <c r="T30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
-      <c r="U30" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U30" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -4542,27 +4551,27 @@
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44773</v>
       </c>
       <c r="K31" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/07/2022</v>
       </c>
       <c r="L31" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>31/07/2022</v>
       </c>
       <c r="M31" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5 - MCE - 202207 - 20074827455 - SZYCHOWSKI RICARDO</v>
       </c>
       <c r="N31" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5 - MCR - 202207 - 20074827455 - SZYCHOWSKI RICARDO</v>
       </c>
       <c r="O31" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P31" s="1" t="e">
@@ -4570,7 +4579,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q31" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R31" s="7" t="s">
@@ -4580,11 +4589,11 @@
         <v>2</v>
       </c>
       <c r="T31" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>31</v>
       </c>
-      <c r="U31" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U31" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202207</v>
       </c>
     </row>
@@ -4612,27 +4621,27 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K32" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L32" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M32" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5 - MCE - 202302 - 20170394845 - FERREYRA MARCELO JORGE</v>
       </c>
       <c r="N32" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5 - MCR - 202302 - 20170394845 - FERREYRA MARCELO JORGE</v>
       </c>
       <c r="O32" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P32" s="1" t="e">
@@ -4640,7 +4649,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q32" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R32" s="7" t="s">
@@ -4650,11 +4659,11 @@
         <v>2</v>
       </c>
       <c r="T32" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>32</v>
       </c>
-      <c r="U32" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U32" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
@@ -4682,27 +4691,27 @@
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K33" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L33" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M33" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5 - MCE - 202302 - 27148268105 - CANTELI GRACIELA</v>
       </c>
       <c r="N33" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>5 - MCR - 202302 - 27148268105 - CANTELI GRACIELA</v>
       </c>
       <c r="O33" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P33" s="1" t="e">
@@ -4710,7 +4719,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q33" s="6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R33" s="7" t="s">
@@ -4720,17 +4729,17 @@
         <v>2</v>
       </c>
       <c r="T33" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>33</v>
       </c>
-      <c r="U33" s="1" t="str">
-        <f t="shared" si="9"/>
+      <c r="U33" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
-        <f t="shared" ref="A34:A69" si="10">RIGHT(D34,1)</f>
+        <f t="shared" ref="A34:A69" si="14">RIGHT(D34,1)</f>
         <v>5</v>
       </c>
       <c r="B34" t="s">
@@ -4752,27 +4761,27 @@
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="3">
-        <f t="shared" ref="J34:J69" si="11">EOMONTH(F34,0)</f>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K34" s="3" t="str">
-        <f t="shared" ref="K34:K69" si="12">TEXT(F34,"DD/MM/AAAA")</f>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L34" s="3" t="str">
-        <f t="shared" ref="L34:L69" si="13">TEXT(J34,"DD/MM/AAAA")</f>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M34" s="3" t="str">
-        <f t="shared" ref="M34:M69" si="14">CONCATENATE(A34," - ","MCE - ",TEXT(K34,"AAAAMM")," - ",SUBSTITUTE(D34,"-","")," - ",B34)</f>
+        <f t="shared" si="8"/>
         <v>5 - MCE - 202302 - 27171709925 - CORONAS ALINE</v>
       </c>
       <c r="N34" s="3" t="str">
-        <f t="shared" ref="N34:N69" si="15">CONCATENATE(A34," - ","MCR - ",TEXT(K34,"AAAAMM")," - ",SUBSTITUTE(D34,"-","")," - ",B34)</f>
+        <f t="shared" si="9"/>
         <v>5 - MCR - 202302 - 27171709925 - CORONAS ALINE</v>
       </c>
       <c r="O34" s="1" t="str">
-        <f t="shared" ref="O34:O69" si="16">TEXT(R34+S34/96400,"hh:mm:ss")</f>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P34" s="1" t="e">
@@ -4780,7 +4789,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q34" s="6" t="e">
-        <f t="shared" ref="Q34:Q65" si="17">IF(EXACT(P34,E34),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R34" s="7" t="s">
@@ -4790,17 +4799,17 @@
         <v>2</v>
       </c>
       <c r="T34" s="1">
-        <f t="shared" ref="T34:T69" si="18">ROW(A34)</f>
+        <f t="shared" si="12"/>
         <v>34</v>
       </c>
-      <c r="U34" s="1" t="str">
-        <f t="shared" ref="U34:U69" si="19">TEXT(K34,"AAAAMM")</f>
+      <c r="U34" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="B35" t="s">
@@ -4821,27 +4830,27 @@
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K35" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L35" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M35" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>6 - MCE - 202302 - 20149466356 - ENRIQUEZ RUBEN</v>
       </c>
       <c r="N35" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>6 - MCR - 202302 - 20149466356 - ENRIQUEZ RUBEN</v>
       </c>
       <c r="O35" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P35" s="1" t="e">
@@ -4849,7 +4858,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q35" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R35" s="7" t="s">
@@ -4859,17 +4868,17 @@
         <v>2</v>
       </c>
       <c r="T35" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>35</v>
       </c>
-      <c r="U35" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U35" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="B36" t="s">
@@ -4890,27 +4899,27 @@
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K36" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L36" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M36" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>6 - MCE - 202302 - 20416948926 - BEITIA IÑAKI</v>
       </c>
       <c r="N36" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>6 - MCR - 202302 - 20416948926 - BEITIA IÑAKI</v>
       </c>
       <c r="O36" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P36" s="1" t="e">
@@ -4918,7 +4927,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q36" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R36" s="7" t="s">
@@ -4928,17 +4937,17 @@
         <v>2</v>
       </c>
       <c r="T36" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>36</v>
       </c>
-      <c r="U36" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U36" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="B37" t="s">
@@ -4960,27 +4969,27 @@
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K37" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L37" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M37" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">6 - MCE - 202302 - 27201178776 - SZYCHOWSKI AMANDA </v>
       </c>
       <c r="N37" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">6 - MCR - 202302 - 27201178776 - SZYCHOWSKI AMANDA </v>
       </c>
       <c r="O37" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P37" s="1" t="e">
@@ -4988,7 +4997,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q37" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R37" s="7" t="s">
@@ -4998,17 +5007,17 @@
         <v>2</v>
       </c>
       <c r="T37" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
-      <c r="U37" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U37" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="B38" t="s">
@@ -5030,27 +5039,27 @@
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K38" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L38" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M38" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>6 - MCE - 202302 - 27261827366 - CARBALLO GRACELA</v>
       </c>
       <c r="N38" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>6 - MCR - 202302 - 27261827366 - CARBALLO GRACELA</v>
       </c>
       <c r="O38" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P38" s="1" t="e">
@@ -5058,7 +5067,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q38" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R38" s="7" t="s">
@@ -5068,17 +5077,17 @@
         <v>2</v>
       </c>
       <c r="T38" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>38</v>
       </c>
-      <c r="U38" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U38" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="B39" t="s">
@@ -5099,27 +5108,27 @@
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K39" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L39" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M39" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>6 - MCE - 202302 - 30715347926 - CONSULTORIO SAN MARTIN</v>
       </c>
       <c r="N39" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>6 - MCR - 202302 - 30715347926 - CONSULTORIO SAN MARTIN</v>
       </c>
       <c r="O39" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P39" s="1" t="e">
@@ -5127,7 +5136,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q39" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R39" s="7" t="s">
@@ -5137,17 +5146,17 @@
         <v>2</v>
       </c>
       <c r="T39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>39</v>
       </c>
-      <c r="U39" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U39" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="B40" t="s">
@@ -5168,27 +5177,27 @@
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K40" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L40" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M40" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>6 - MCE - 202302 - 30716503816 - PENSA PROPIEDADES</v>
       </c>
       <c r="N40" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>6 - MCR - 202302 - 30716503816 - PENSA PROPIEDADES</v>
       </c>
       <c r="O40" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P40" s="1" t="e">
@@ -5196,7 +5205,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q40" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R40" s="7" t="s">
@@ -5206,17 +5215,17 @@
         <v>2</v>
       </c>
       <c r="T40" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
-      <c r="U40" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U40" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B41" t="s">
@@ -5226,7 +5235,7 @@
         <v>20077065637</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" ref="D41:D48" si="20">TEXT(C41,"00-00000000-0")</f>
+        <f t="shared" ref="D41:D48" si="15">TEXT(C41,"00-00000000-0")</f>
         <v>20-07706563-7</v>
       </c>
       <c r="F41" s="4">
@@ -5238,27 +5247,27 @@
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K41" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L41" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M41" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 20077065637 - PENSA ANIBAL</v>
       </c>
       <c r="N41" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 20077065637 - PENSA ANIBAL</v>
       </c>
       <c r="O41" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P41" s="1" t="e">
@@ -5266,7 +5275,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q41" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R41" s="7" t="s">
@@ -5276,17 +5285,17 @@
         <v>2</v>
       </c>
       <c r="T41" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>41</v>
       </c>
-      <c r="U41" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U41" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B42" t="s">
@@ -5296,7 +5305,7 @@
         <v>20130056637</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>20-13005663-7</v>
       </c>
       <c r="F42" s="4">
@@ -5308,27 +5317,27 @@
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K42" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L42" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M42" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 20130056637 - TABBIA ENRIQUE</v>
       </c>
       <c r="N42" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 20130056637 - TABBIA ENRIQUE</v>
       </c>
       <c r="O42" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P42" s="1" t="e">
@@ -5336,7 +5345,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q42" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R42" s="7" t="s">
@@ -5346,17 +5355,17 @@
         <v>2</v>
       </c>
       <c r="T42" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>42</v>
       </c>
-      <c r="U42" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U42" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B43" t="s">
@@ -5366,7 +5375,7 @@
         <v>20170395167</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>20-17039516-7</v>
       </c>
       <c r="F43" s="4">
@@ -5378,27 +5387,27 @@
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K43" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L43" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M43" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 20170395167 - HOPE HUGO</v>
       </c>
       <c r="N43" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 20170395167 - HOPE HUGO</v>
       </c>
       <c r="O43" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P43" s="1" t="e">
@@ -5406,7 +5415,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q43" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R43" s="7" t="s">
@@ -5416,17 +5425,17 @@
         <v>2</v>
       </c>
       <c r="T43" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>43</v>
       </c>
-      <c r="U43" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U43" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B44" t="s">
@@ -5436,7 +5445,7 @@
         <v>20301650087</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>20-30165008-7</v>
       </c>
       <c r="F44" s="4">
@@ -5448,27 +5457,27 @@
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K44" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L44" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M44" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 20301650087 - VARENIZA NESTOR LEONEL</v>
       </c>
       <c r="N44" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 20301650087 - VARENIZA NESTOR LEONEL</v>
       </c>
       <c r="O44" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P44" s="1" t="e">
@@ -5476,7 +5485,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q44" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R44" s="7" t="s">
@@ -5486,17 +5495,17 @@
         <v>2</v>
       </c>
       <c r="T44" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>44</v>
       </c>
-      <c r="U44" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U44" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B45" t="s">
@@ -5506,7 +5515,7 @@
         <v>20327623967</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>20-32762396-7</v>
       </c>
       <c r="F45" s="4">
@@ -5518,27 +5527,27 @@
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K45" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L45" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M45" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 20327623967 - FERREYRA CARLOS ANDRES</v>
       </c>
       <c r="N45" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 20327623967 - FERREYRA CARLOS ANDRES</v>
       </c>
       <c r="O45" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P45" s="1" t="e">
@@ -5546,7 +5555,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q45" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R45" s="7" t="s">
@@ -5556,17 +5565,17 @@
         <v>2</v>
       </c>
       <c r="T45" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
-      <c r="U45" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U45" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B46" t="s">
@@ -5576,7 +5585,7 @@
         <v>20334250327</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>20-33425032-7</v>
       </c>
       <c r="E46" t="s">
@@ -5594,27 +5603,27 @@
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44773</v>
       </c>
       <c r="K46" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/07/2022</v>
       </c>
       <c r="L46" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>31/07/2022</v>
       </c>
       <c r="M46" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202207 - 20334250327 - PENSA LUCIANO ANIBAL</v>
       </c>
       <c r="N46" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202207 - 20334250327 - PENSA LUCIANO ANIBAL</v>
       </c>
       <c r="O46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P46" s="1" t="e">
@@ -5622,7 +5631,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q46" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R46" s="7" t="s">
@@ -5632,17 +5641,17 @@
         <v>2</v>
       </c>
       <c r="T46" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>46</v>
       </c>
-      <c r="U46" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U46" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202207</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B47" t="s">
@@ -5652,7 +5661,7 @@
         <v>27109797257</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>27-10979725-7</v>
       </c>
       <c r="F47" s="4">
@@ -5664,27 +5673,27 @@
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K47" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L47" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M47" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 27109797257 - SCOTTO OLGA MARIA</v>
       </c>
       <c r="N47" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 27109797257 - SCOTTO OLGA MARIA</v>
       </c>
       <c r="O47" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P47" s="1" t="e">
@@ -5692,7 +5701,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q47" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R47" s="7" t="s">
@@ -5702,17 +5711,17 @@
         <v>2</v>
       </c>
       <c r="T47" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>47</v>
       </c>
-      <c r="U47" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U47" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B48" t="s">
@@ -5722,7 +5731,7 @@
         <v>27217236547</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>27-21723654-7</v>
       </c>
       <c r="F48" s="4">
@@ -5734,27 +5743,27 @@
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K48" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L48" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M48" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 27217236547 - ROKO MARIA EUGENIA</v>
       </c>
       <c r="N48" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 27217236547 - ROKO MARIA EUGENIA</v>
       </c>
       <c r="O48" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P48" s="1" t="e">
@@ -5762,7 +5771,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q48" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R48" s="7" t="s">
@@ -5772,17 +5781,17 @@
         <v>2</v>
       </c>
       <c r="T48" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>48</v>
       </c>
-      <c r="U48" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U48" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B49" t="s">
@@ -5803,27 +5812,27 @@
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K49" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L49" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M49" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 30650940667 - BUSTOS-HOPE S.H</v>
       </c>
       <c r="N49" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 30650940667 - BUSTOS-HOPE S.H</v>
       </c>
       <c r="O49" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P49" s="1" t="e">
@@ -5831,7 +5840,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q49" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R49" s="7" t="s">
@@ -5841,17 +5850,17 @@
         <v>2</v>
       </c>
       <c r="T49" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>49</v>
       </c>
-      <c r="U49" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U49" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B50" t="s">
@@ -5878,27 +5887,27 @@
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44773</v>
       </c>
       <c r="K50" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/07/2022</v>
       </c>
       <c r="L50" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>31/07/2022</v>
       </c>
       <c r="M50" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202207 - 30672372697 - CEBAC</v>
       </c>
       <c r="N50" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202207 - 30672372697 - CEBAC</v>
       </c>
       <c r="O50" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P50" s="1" t="e">
@@ -5906,7 +5915,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q50" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R50" s="7" t="s">
@@ -5916,17 +5925,17 @@
         <v>2</v>
       </c>
       <c r="T50" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
-      <c r="U50" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U50" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202207</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B51" t="s">
@@ -5947,27 +5956,27 @@
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K51" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L51" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M51" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 30709419567 - AITA S.A.</v>
       </c>
       <c r="N51" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 30709419567 - AITA S.A.</v>
       </c>
       <c r="O51" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P51" s="1" t="e">
@@ -5975,7 +5984,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q51" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R51" s="7" t="s">
@@ -5985,17 +5994,17 @@
         <v>2</v>
       </c>
       <c r="T51" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>51</v>
       </c>
-      <c r="U51" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U51" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="B52" t="s">
@@ -6016,27 +6025,27 @@
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K52" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L52" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M52" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>7 - MCE - 202302 - 30712026797 - COND. LARZABAL</v>
       </c>
       <c r="N52" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>7 - MCR - 202302 - 30712026797 - COND. LARZABAL</v>
       </c>
       <c r="O52" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P52" s="1" t="e">
@@ -6044,7 +6053,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q52" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R52" s="7" t="s">
@@ -6054,17 +6063,17 @@
         <v>2</v>
       </c>
       <c r="T52" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>52</v>
       </c>
-      <c r="U52" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U52" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B53" t="s">
@@ -6086,27 +6095,27 @@
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K53" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L53" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M53" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>8 - MCE - 202302 - 20082750488 - CASTRO OLIVERA CARLOS</v>
       </c>
       <c r="N53" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>8 - MCR - 202302 - 20082750488 - CASTRO OLIVERA CARLOS</v>
       </c>
       <c r="O53" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P53" s="1" t="e">
@@ -6114,7 +6123,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q53" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R53" s="7" t="s">
@@ -6124,17 +6133,17 @@
         <v>2</v>
       </c>
       <c r="T53" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>53</v>
       </c>
-      <c r="U53" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U53" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B54" t="s">
@@ -6156,27 +6165,27 @@
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K54" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L54" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M54" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>8 - MCE - 202302 - 20230966738 - URRUTIA DIEGO</v>
       </c>
       <c r="N54" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>8 - MCR - 202302 - 20230966738 - URRUTIA DIEGO</v>
       </c>
       <c r="O54" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P54" s="1" t="e">
@@ -6184,7 +6193,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q54" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R54" s="7" t="s">
@@ -6194,17 +6203,17 @@
         <v>2</v>
       </c>
       <c r="T54" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>54</v>
       </c>
-      <c r="U54" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U54" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B55" t="s">
@@ -6226,27 +6235,27 @@
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K55" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L55" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M55" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>8 - MCE - 202302 - 20303980378 - CASTRO OLIVERA GONZALO</v>
       </c>
       <c r="N55" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>8 - MCR - 202302 - 20303980378 - CASTRO OLIVERA GONZALO</v>
       </c>
       <c r="O55" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P55" s="1" t="e">
@@ -6254,7 +6263,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q55" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R55" s="7" t="s">
@@ -6264,17 +6273,17 @@
         <v>2</v>
       </c>
       <c r="T55" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>55</v>
       </c>
-      <c r="U55" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U55" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B56" t="s">
@@ -6296,27 +6305,27 @@
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K56" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L56" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M56" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>8 - MCE - 202302 - 27163651918 - MARTIN MONICA ADRIANA</v>
       </c>
       <c r="N56" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>8 - MCR - 202302 - 27163651918 - MARTIN MONICA ADRIANA</v>
       </c>
       <c r="O56" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P56" s="1" t="e">
@@ -6324,7 +6333,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q56" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R56" s="7" t="s">
@@ -6334,17 +6343,17 @@
         <v>2</v>
       </c>
       <c r="T56" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>56</v>
       </c>
-      <c r="U56" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U56" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B57" t="s">
@@ -6366,27 +6375,27 @@
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K57" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L57" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M57" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>8 - MCE - 202302 - 27201932268 - SPAGNOLI SUSANA</v>
       </c>
       <c r="N57" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>8 - MCR - 202302 - 27201932268 - SPAGNOLI SUSANA</v>
       </c>
       <c r="O57" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P57" s="1" t="e">
@@ -6394,7 +6403,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q57" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R57" s="7" t="s">
@@ -6404,17 +6413,17 @@
         <v>2</v>
       </c>
       <c r="T57" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>57</v>
       </c>
-      <c r="U57" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U57" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B58" t="s">
@@ -6435,27 +6444,27 @@
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K58" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L58" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M58" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>8 - MCE - 202302 - 30701299538 - FORESTAL SA</v>
       </c>
       <c r="N58" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>8 - MCR - 202302 - 30701299538 - FORESTAL SA</v>
       </c>
       <c r="O58" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P58" s="1" t="e">
@@ -6463,7 +6472,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q58" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R58" s="7" t="s">
@@ -6473,17 +6482,17 @@
         <v>2</v>
       </c>
       <c r="T58" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>58</v>
       </c>
-      <c r="U58" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U58" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="B59" t="s">
@@ -6504,27 +6513,27 @@
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K59" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L59" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M59" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>8 - MCE - 202302 - 30708626348 - FIDEIC. PDAS INMOB</v>
       </c>
       <c r="N59" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>8 - MCR - 202302 - 30708626348 - FIDEIC. PDAS INMOB</v>
       </c>
       <c r="O59" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P59" s="1" t="e">
@@ -6532,7 +6541,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q59" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R59" s="7" t="s">
@@ -6542,17 +6551,17 @@
         <v>2</v>
       </c>
       <c r="T59" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>59</v>
       </c>
-      <c r="U59" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U59" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B60" t="s">
@@ -6574,27 +6583,27 @@
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K60" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L60" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M60" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>9 - MCE - 202302 - 20149466739 - HOPE RICARDO MARIO</v>
       </c>
       <c r="N60" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>9 - MCR - 202302 - 20149466739 - HOPE RICARDO MARIO</v>
       </c>
       <c r="O60" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P60" s="1" t="e">
@@ -6602,7 +6611,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q60" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R60" s="7" t="s">
@@ -6612,17 +6621,17 @@
         <v>2</v>
       </c>
       <c r="T60" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
-      <c r="U60" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U60" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B61" t="s">
@@ -6643,27 +6652,27 @@
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K61" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L61" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M61" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>9 - MCE - 202302 - 20175255819 - BEITIA CRISPIN</v>
       </c>
       <c r="N61" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>9 - MCR - 202302 - 20175255819 - BEITIA CRISPIN</v>
       </c>
       <c r="O61" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P61" s="1" t="e">
@@ -6671,7 +6680,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q61" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R61" s="7" t="s">
@@ -6681,17 +6690,17 @@
         <v>2</v>
       </c>
       <c r="T61" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>61</v>
       </c>
-      <c r="U61" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U61" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B62" t="s">
@@ -6716,27 +6725,27 @@
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K62" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L62" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M62" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>9 - MCE - 202302 - 20246008109 - BUSTOS GONZALO</v>
       </c>
       <c r="N62" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>9 - MCR - 202302 - 20246008109 - BUSTOS GONZALO</v>
       </c>
       <c r="O62" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P62" s="1" t="e">
@@ -6744,7 +6753,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q62" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R62" s="7" t="s">
@@ -6754,17 +6763,17 @@
         <v>2</v>
       </c>
       <c r="T62" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>62</v>
       </c>
-      <c r="U62" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U62" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B63" t="s">
@@ -6786,27 +6795,27 @@
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K63" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L63" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M63" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>9 - MCE - 202302 - 23120538209 - LINDSTROM PLINIO</v>
       </c>
       <c r="N63" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>9 - MCR - 202302 - 23120538209 - LINDSTROM PLINIO</v>
       </c>
       <c r="O63" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P63" s="1" t="e">
@@ -6814,7 +6823,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q63" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R63" s="7" t="s">
@@ -6824,17 +6833,17 @@
         <v>2</v>
       </c>
       <c r="T63" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>63</v>
       </c>
-      <c r="U63" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U63" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B64" t="s">
@@ -6856,27 +6865,27 @@
       </c>
       <c r="I64" s="2"/>
       <c r="J64" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K64" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L64" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M64" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>9 - MCE - 202302 - 23242946669 - SOTO MIGUEL GERONIMO</v>
       </c>
       <c r="N64" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>9 - MCR - 202302 - 23242946669 - SOTO MIGUEL GERONIMO</v>
       </c>
       <c r="O64" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P64" s="1" t="e">
@@ -6884,7 +6893,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q64" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R64" s="7" t="s">
@@ -6894,17 +6903,17 @@
         <v>2</v>
       </c>
       <c r="T64" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>64</v>
       </c>
-      <c r="U64" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U64" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B65" t="s">
@@ -6920,27 +6929,27 @@
         <v>44958</v>
       </c>
       <c r="J65" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K65" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L65" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M65" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>9 - MCE - 202302 - 27173878309 - LIONETTO ANA CAROLINA</v>
       </c>
       <c r="N65" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>9 - MCR - 202302 - 27173878309 - LIONETTO ANA CAROLINA</v>
       </c>
       <c r="O65" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P65" s="1" t="e">
@@ -6948,7 +6957,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q65" s="6" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R65" s="7" t="s">
@@ -6958,17 +6967,17 @@
         <v>2</v>
       </c>
       <c r="T65" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>65</v>
       </c>
-      <c r="U65" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U65" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B66" t="s">
@@ -6989,27 +6998,27 @@
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>44985</v>
       </c>
       <c r="K66" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>01/02/2023</v>
       </c>
       <c r="L66" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v>28/02/2023</v>
       </c>
       <c r="M66" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v>9 - MCE - 202302 - 30715085409 - COND. INVERNADA</v>
       </c>
       <c r="N66" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>9 - MCR - 202302 - 30715085409 - COND. INVERNADA</v>
       </c>
       <c r="O66" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>00:00:03</v>
       </c>
       <c r="P66" s="1" t="e">
@@ -7017,7 +7026,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q66" s="6" t="e">
-        <f t="shared" ref="Q66:Q69" si="21">IF(EXACT(P66,E66),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="R66" s="7" t="s">
@@ -7027,17 +7036,17 @@
         <v>2</v>
       </c>
       <c r="T66" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>66</v>
       </c>
-      <c r="U66" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U66" s="3" t="str">
+        <f t="shared" si="13"/>
         <v>202302</v>
       </c>
     </row>
     <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B67" t="s">
@@ -7064,27 +7073,27 @@
       </c>
       <c r="I67" s="2"/>
       <c r="J67" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="J67:J69" si="16">EOMONTH(F67,0)</f>
         <v>44773</v>
       </c>
       <c r="K67" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="K67:K69" si="17">TEXT(DAY(F67),"00")&amp;"/"&amp;TEXT(MONTH(F67),"00")&amp;"/"&amp;YEAR(F67)</f>
         <v>01/07/2022</v>
       </c>
       <c r="L67" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L67:L69" si="18">TEXT(DAY(J67),"00")&amp;"/"&amp;TEXT(MONTH(J67),"00")&amp;"/"&amp;YEAR(J67)</f>
         <v>31/07/2022</v>
       </c>
       <c r="M67" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="M67:M69" si="19">CONCATENATE(A67," - ","MCE - ",U67," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
         <v>9 - MCE - 202207 - 33653520439 - FAX SRL</v>
       </c>
       <c r="N67" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="N67:N69" si="20">CONCATENATE(A67," - ","MCR - ",U67," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
         <v>9 - MCR - 202207 - 33653520439 - FAX SRL</v>
       </c>
       <c r="O67" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="O67:O69" si="21">TEXT(R67+S67/96400,"hh:mm:ss")</f>
         <v>00:00:03</v>
       </c>
       <c r="P67" s="1" t="e">
@@ -7092,7 +7101,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q67" s="6" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="Q67:Q69" si="22">IF(EXACT(P67,E67),"ü","x")</f>
         <v>#N/A</v>
       </c>
       <c r="R67" s="7" t="s">
@@ -7102,17 +7111,17 @@
         <v>2</v>
       </c>
       <c r="T67" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="T67:T69" si="23">ROW(A67)</f>
         <v>67</v>
       </c>
-      <c r="U67" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U67" s="3" t="str">
+        <f t="shared" ref="U67:U69" si="24">YEAR(F67)&amp;TEXT(MONTH(F67),"00")</f>
         <v>202207</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B68" t="s">
@@ -7133,27 +7142,27 @@
       </c>
       <c r="I68" s="2"/>
       <c r="J68" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>44985</v>
       </c>
       <c r="K68" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>01/02/2023</v>
       </c>
       <c r="L68" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>28/02/2023</v>
       </c>
       <c r="M68" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>9 - MCE - 202302 - 33712370829 - KM 0 SA</v>
       </c>
       <c r="N68" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>9 - MCR - 202302 - 33712370829 - KM 0 SA</v>
       </c>
       <c r="O68" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>00:00:03</v>
       </c>
       <c r="P68" s="1" t="e">
@@ -7161,7 +7170,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q68" s="6" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>#N/A</v>
       </c>
       <c r="R68" s="7" t="s">
@@ -7171,17 +7180,17 @@
         <v>2</v>
       </c>
       <c r="T68" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>68</v>
       </c>
-      <c r="U68" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U68" s="3" t="str">
+        <f t="shared" si="24"/>
         <v>202302</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="B69" t="s">
@@ -7202,27 +7211,27 @@
       </c>
       <c r="I69" s="2"/>
       <c r="J69" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>44985</v>
       </c>
       <c r="K69" s="3" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>01/02/2023</v>
       </c>
       <c r="L69" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>28/02/2023</v>
       </c>
       <c r="M69" s="3" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>9 - MCE - 202302 - 33712529909 - INMUEBLES SRL</v>
       </c>
       <c r="N69" s="3" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>9 - MCR - 202302 - 33712529909 - INMUEBLES SRL</v>
       </c>
       <c r="O69" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>00:00:03</v>
       </c>
       <c r="P69" s="1" t="e">
@@ -7230,7 +7239,7 @@
         <v>#N/A</v>
       </c>
       <c r="Q69" s="6" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>#N/A</v>
       </c>
       <c r="R69" s="7" t="s">
@@ -7240,11 +7249,11 @@
         <v>2</v>
       </c>
       <c r="T69" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>69</v>
       </c>
-      <c r="U69" s="1" t="str">
-        <f t="shared" si="19"/>
+      <c r="U69" s="3" t="str">
+        <f t="shared" si="24"/>
         <v>202302</v>
       </c>
     </row>

</xml_diff>